<commit_message>
copy exclusion template from prod
</commit_message>
<xml_diff>
--- a/Projects/JNJUK_SAND/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJUK_SAND/Data/KPI Exclusions Template.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">All</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub Category </t>
+    <t xml:space="preserve">sub_category</t>
   </si>
   <si>
     <t xml:space="preserve">COLD &amp; FLU ; IBS ; KIDS COLD &amp; FLU ; COLD &amp; FLU ;KIDS COUGH ; KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH ; KIDS HAYFEVER ; LAXATIVES ; KIDS TEETHING ; WIND ; ALLERGY ; REHYDRATION ; PROBIOTICS ; PAIN MANAGEMENT ; ANTI-AGE FACE ; ARTIFICIAL TAN ; BODY CLEANSING ; BODY SPRAY ; COSMETICS ; DEODORANTS ; MEN'S TOILETRIES ; SUNCARE ; HAIR CARE ;  BABY HEALTHCARE ; FOR MUM ; KIDS HAIRCARE ; KIDS TOILETRIES ;  KIDS WIPES ; COTTON ; INCONTINENCE ; SANITARY TOWELS ; FEMININE WASH ; KIDS MOUTHWASH </t>
@@ -301,17 +301,17 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0971659919028"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3036437246964"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="206.769230769231"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6882591093117"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2591093117409"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="208.668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>